<commit_message>
Changes to support clock wise and anti clock wise rotation
</commit_message>
<xml_diff>
--- a/PictureManager/Documents/picturemoduleFinal_Usecases.xlsx
+++ b/PictureManager/Documents/picturemoduleFinal_Usecases.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="123820"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
   <si>
     <t>Run Application when there is no network connection</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Aspect ratio is never changed!!</t>
-  </si>
-  <si>
     <t>Intelligent scaling!!</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
   </si>
   <si>
     <t>iOS only</t>
-  </si>
-  <si>
-    <t>In ios only landscape to portrait rotation supported</t>
   </si>
   <si>
     <t xml:space="preserve">both iOS/Android </t>
@@ -317,19 +311,22 @@
 Then user should be able to see correct compressed image to the specified scale value
   </t>
   </si>
+  <si>
+    <t>Known issue :On iOS  aspect ratio is not propers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -563,16 +560,16 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -608,10 +605,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,6 +683,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -700,12 +703,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -869,7 +866,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -904,7 +900,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1077,17 +1072,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="7" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1096,7 +1091,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1105,7 +1100,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1114,29 +1109,29 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+    <row r="4" spans="1:7" ht="15" customHeight="1">
+      <c r="A4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-    </row>
-    <row r="5" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+    </row>
+    <row r="5" spans="1:7" ht="23.25">
+      <c r="A5" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1145,7 +1140,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1154,18 +1149,18 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+    <row r="8" spans="1:7" ht="15" customHeight="1">
+      <c r="A8" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1174,7 +1169,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1183,7 +1178,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1192,7 +1187,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1201,7 +1196,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1210,7 +1205,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1219,7 +1214,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1228,7 +1223,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1237,7 +1232,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1246,7 +1241,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1255,7 +1250,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1264,7 +1259,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1285,12 +1280,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="3" width="35.28515625" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
@@ -1300,7 +1295,7 @@
     <col min="8" max="8" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1310,7 +1305,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1334,7 +1329,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
@@ -1358,7 +1353,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -1382,7 +1377,7 @@
       </c>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1406,7 +1401,7 @@
       </c>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1430,7 +1425,7 @@
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
@@ -1452,7 +1447,7 @@
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -1462,7 +1457,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1472,7 +1467,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1482,7 +1477,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1492,7 +1487,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1502,7 +1497,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1512,7 +1507,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1522,7 +1517,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1532,7 +1527,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1542,7 +1537,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1552,7 +1547,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1562,7 +1557,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1572,7 +1567,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1589,14 +1584,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="3" width="55.140625" customWidth="1"/>
@@ -1605,7 +1600,7 @@
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="16" t="s">
         <v>35</v>
       </c>
@@ -1619,14 +1614,14 @@
         <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>64</v>
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -1634,17 +1629,17 @@
         <v>39</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="36"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -1652,37 +1647,35 @@
         <v>6</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="88.5" customHeight="1">
       <c r="A4" s="35">
         <v>3</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="45" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>65</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D4" s="42"/>
       <c r="E4" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="27.75" customHeight="1">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -1690,17 +1683,17 @@
         <v>60</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="36"/>
     </row>
-    <row r="6" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="45.75" customHeight="1">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -1708,17 +1701,17 @@
         <v>48</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" s="36"/>
     </row>
-    <row r="7" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="55.5" customHeight="1">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -1726,17 +1719,17 @@
         <v>41</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="36" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7" s="36"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="15"/>
       <c r="B8" s="43"/>
       <c r="C8" s="15"/>
@@ -1744,7 +1737,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1752,7 +1745,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1760,7 +1753,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1768,7 +1761,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1776,7 +1769,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1784,22 +1777,22 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" customHeight="1">
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1">
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" ht="15" customHeight="1">
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" ht="15" customHeight="1">
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6" ht="15" customHeight="1">
       <c r="F19" s="1"/>
     </row>
   </sheetData>
@@ -1809,14 +1802,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="79.42578125" bestFit="1" customWidth="1"/>
@@ -1825,7 +1818,7 @@
     <col min="5" max="7" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -1833,7 +1826,7 @@
         <v>56</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>15</v>
@@ -1842,69 +1835,69 @@
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
     </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="75">
       <c r="A2" s="36">
         <v>1</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="60">
       <c r="A3" s="36">
         <v>2</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
     </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="75">
       <c r="A4" s="23">
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" s="44"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="60">
       <c r="A5" s="23">
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="75">
       <c r="A6" s="36">
         <v>15</v>
       </c>
@@ -1912,46 +1905,46 @@
         <v>49</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="75">
       <c r="A7" s="23">
         <v>16</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="51" t="s">
-        <v>66</v>
+        <v>75</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>65</v>
       </c>
       <c r="E7" s="40"/>
       <c r="F7" s="41"/>
       <c r="G7" s="41"/>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60">
       <c r="A8" s="23">
         <v>17</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
       <c r="G8" s="39"/>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60">
       <c r="A9" s="23">
         <v>22</v>
       </c>
@@ -1959,7 +1952,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="38"/>
@@ -1973,19 +1966,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="96.42578125" customWidth="1"/>
     <col min="3" max="6" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="26" t="s">
         <v>35</v>
       </c>
@@ -1997,7 +1990,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -2009,7 +2002,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="28">
         <v>2</v>
       </c>
@@ -2021,7 +2014,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="27">
         <v>3</v>
       </c>
@@ -2033,7 +2026,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="27"/>
       <c r="B5" s="27"/>
       <c r="C5" s="17"/>
@@ -2041,7 +2034,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="28"/>
       <c r="B6" s="28"/>
       <c r="C6" s="17"/>
@@ -2049,7 +2042,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="1"/>
@@ -2057,7 +2050,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2065,7 +2058,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2073,7 +2066,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2081,7 +2074,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2089,7 +2082,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2097,7 +2090,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2105,7 +2098,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2113,7 +2106,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2121,7 +2114,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2129,7 +2122,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2137,7 +2130,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2145,7 +2138,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2153,7 +2146,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2168,12 +2161,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="55.140625" customWidth="1"/>
@@ -2182,19 +2175,19 @@
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="51"/>
       <c r="C1" s="29"/>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="49"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
@@ -2210,7 +2203,7 @@
       </c>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="23">
         <v>1</v>
       </c>
@@ -2226,7 +2219,7 @@
       </c>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="23">
         <v>2</v>
       </c>
@@ -2242,7 +2235,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="23">
         <v>3</v>
       </c>
@@ -2256,7 +2249,7 @@
       <c r="E5" s="34"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="23">
         <v>4</v>
       </c>
@@ -2270,7 +2263,7 @@
       <c r="E6" s="34"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="23">
         <v>5</v>
       </c>
@@ -2282,7 +2275,7 @@
       <c r="E7" s="34"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="23">
         <v>6</v>
       </c>
@@ -2294,7 +2287,7 @@
       <c r="E8" s="34"/>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="23">
         <v>7</v>
       </c>
@@ -2306,7 +2299,7 @@
       <c r="E9" s="35"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="23">
         <v>8</v>
       </c>
@@ -2318,7 +2311,7 @@
       <c r="E10" s="34"/>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="23"/>
       <c r="B11" s="33"/>
       <c r="C11" s="31"/>
@@ -2328,7 +2321,7 @@
       <c r="E11" s="34"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="23"/>
       <c r="B12" s="33"/>
       <c r="C12" s="31"/>
@@ -2338,7 +2331,7 @@
       <c r="E12" s="34"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="23"/>
       <c r="B13" s="33"/>
       <c r="C13" s="31"/>
@@ -2348,7 +2341,7 @@
       <c r="E13" s="34"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="1"/>
@@ -2356,7 +2349,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2364,7 +2357,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2372,7 +2365,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2380,7 +2373,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2388,7 +2381,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2396,7 +2389,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2415,12 +2408,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.140625" customWidth="1"/>
@@ -2428,7 +2421,7 @@
     <col min="5" max="6" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -2442,7 +2435,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -2458,7 +2451,7 @@
       <c r="E2" s="17"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -2470,7 +2463,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -2482,7 +2475,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -2494,7 +2487,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -2506,7 +2499,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -2518,7 +2511,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -2528,7 +2521,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -2538,7 +2531,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -2548,7 +2541,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -2558,7 +2551,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -2566,7 +2559,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2574,7 +2567,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2582,7 +2575,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2590,7 +2583,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2598,7 +2591,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2606,7 +2599,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2614,7 +2607,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2622,7 +2615,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>

</xml_diff>